<commit_message>
added main_vizual, separated classes from main
</commit_message>
<xml_diff>
--- a/data/Data_for_preliminary_aa.xlsx
+++ b/data/Data_for_preliminary_aa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="49">
   <si>
     <t>point_name</t>
   </si>
@@ -144,6 +144,30 @@
   </si>
   <si>
     <t>corr_xy</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>ST5</t>
+  </si>
+  <si>
+    <t>ST6</t>
   </si>
 </sst>
 </file>
@@ -477,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -598,10 +622,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -640,33 +664,24 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -677,10 +692,10 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -700,9 +715,102 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7">
+        <v>-70</v>
+      </c>
+      <c r="D7">
+        <v>-38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8">
+        <v>-56</v>
+      </c>
+      <c r="D8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9">
+        <v>-147</v>
+      </c>
+      <c r="D9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11">
+        <v>-130</v>
+      </c>
+      <c r="D11">
+        <v>163</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
         <v>0</v>
       </c>
     </row>
@@ -714,10 +822,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -805,30 +913,30 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
         <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -845,7 +953,7 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -862,7 +970,7 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -879,21 +987,21 @@
         <v>4</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
@@ -901,16 +1009,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -918,19 +1026,359 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" t="s">
+        <v>46</v>
+      </c>
+      <c r="E32" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove .idea folder from Git tracking
</commit_message>
<xml_diff>
--- a/data/Data_for_preliminary_aa.xlsx
+++ b/data/Data_for_preliminary_aa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instruments" sheetId="3" r:id="rId1"/>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -615,6 +615,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:H1001">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -625,7 +630,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -815,6 +820,18 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F1001">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1001">
+      <formula1>-1</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1001">
+      <formula1>"base, refined, estimated"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -824,8 +841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1382,7 +1399,30 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1001">
+      <formula1>"linear, angular"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Points!$B$2:$B$1001</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1002 E2:E1001</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Instruments!$C$2:$C$1001</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B1001</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>